<commit_message>
Finished 10mm flexor testing
collected data for 10 mm Festo flexor testing.
</commit_message>
<xml_diff>
--- a/Testing_Data/PressureSensorCalibration.xlsx
+++ b/Testing_Data/PressureSensorCalibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4B7B26-6B19-4298-A52F-46DAAE727923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F9DEA9-AC91-4E5B-B6C9-1278FD81A53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27285" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{ED23B71C-6DC7-4F03-A302-FE33CB0246DD}"/>
+    <workbookView xWindow="-21750" yWindow="4125" windowWidth="21600" windowHeight="11385" xr2:uid="{ED23B71C-6DC7-4F03-A302-FE33CB0246DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -239,7 +239,7 @@
                   <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8899999999999997</c:v>
+                  <c:v>4.82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1410,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4.8899999999999997</v>
+        <v>4.82</v>
       </c>
       <c r="B6">
         <v>620</v>

</xml_diff>

<commit_message>
Added data collection runs for pinned knee with fish scale
</commit_message>
<xml_diff>
--- a/Testing_Data/PressureSensorCalibration.xlsx
+++ b/Testing_Data/PressureSensorCalibration.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Miranda\Documents\GitHub\Bipedal_Robot\Testing_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB65284-F004-44F9-9480-572818017A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603BA10D-32A0-491C-A060-A0322F6E94F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{ED23B71C-6DC7-4F03-A302-FE33CB0246DD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED23B71C-6DC7-4F03-A302-FE33CB0246DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,12 +33,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Voltage (V)</t>
   </si>
   <si>
     <t>Pressure (kPA)</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>pressure</t>
+  </si>
+  <si>
+    <t>Sample</t>
   </si>
 </sst>
 </file>
@@ -228,7 +237,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.85</c:v>
+                  <c:v>0.87</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.0099999999999998</c:v>
@@ -237,7 +246,7 @@
                   <c:v>3.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8099999999999996</c:v>
+                  <c:v>4.9400000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,7 +466,390 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9400000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>620</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2BD6-41CE-8E74-4D384B49972E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="265476303"/>
+        <c:axId val="265404607"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="265476303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="265404607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="265404607"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="265476303"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1013,6 +1405,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1046,6 +1954,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E41F6CD-C328-4AD2-960D-010AE46A87B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1351,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07EB23B-8D5C-452B-917B-439C5A6B7860}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,31 +2307,49 @@
     <col min="2" max="2" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="M2">
+        <v>0.87</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2.0099999999999998</v>
       </c>
       <c r="B3">
         <v>200</v>
       </c>
+      <c r="M3">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="N3">
+        <v>620</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3.33</v>
       </c>
@@ -1395,12 +2357,66 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4.8099999999999996</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="B5">
         <v>620</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="N24" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="C25">
+        <f>151.6*B25-117.58</f>
+        <v>631.32399999999996</v>
+      </c>
+      <c r="N25">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="O25">
+        <f>152.33*N25-132.53</f>
+        <v>619.9802000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="C26">
+        <f>151.6*B26-117.58</f>
+        <v>617.67999999999984</v>
+      </c>
+      <c r="N26">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="O26">
+        <f>152.33*N26-132.53</f>
+        <v>606.27050000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran test on 45.5 cm 10mm BPA
ran a test on 45.5 cm 10 mm BPA. Incomplete because Lawrence's part  blew up in my face, again. Data recorded to StraightForceTest.  Pressure sensor recalibrated. Temperature Logging doesn't work as given to me by Lawrence. I found this out after making a more advance copy called Pressure Data, which saves an excel spreadsheet called Pressure_Data. Updated HX711 app to include pressure data. It worked for a while but the bad thing about this app is that it needs to be recalibrated after every time it's started. HX711 library couldn't be found after a while. Maybe the computer just needs to restart.
</commit_message>
<xml_diff>
--- a/Testing_Data/PressureSensorCalibration.xlsx
+++ b/Testing_Data/PressureSensorCalibration.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Miranda\Documents\GitHub\Bipedal_Robot\Testing_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF611A2E-33F4-4909-B3F9-9EC5179DDE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73AA9C0-E8F7-4A08-8093-309074EF8F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED23B71C-6DC7-4F03-A302-FE33CB0246DD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED23B71C-6DC7-4F03-A302-FE33CB0246DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -232,71 +232,65 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:f>Sheet1!$A$2:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.84</c:v>
+                  <c:v>0.83579999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.29</c:v>
+                  <c:v>1.4467000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.56</c:v>
+                  <c:v>2.0771999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0499999999999998</c:v>
+                  <c:v>2.7517</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.71</c:v>
+                  <c:v>3.3969</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.32</c:v>
+                  <c:v>4.0274000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.04</c:v>
+                  <c:v>4.6627999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.75</c:v>
+                  <c:v>4.8094000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>300</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>400</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>620</c:v>
                 </c:pt>
               </c:numCache>
@@ -622,10 +616,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.84</c:v>
+                  <c:v>0.83579999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.75</c:v>
+                  <c:v>4.8094000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2325,10 +2319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07EB23B-8D5C-452B-917B-439C5A6B7860}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,13 +2347,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.84</v>
+        <v>0.83579999999999999</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0.84</v>
+        <v>0.83579999999999999</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2367,13 +2361,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.29</v>
+        <v>1.4467000000000001</v>
       </c>
       <c r="B3">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="M3">
-        <v>4.75</v>
+        <v>4.8094000000000001</v>
       </c>
       <c r="N3">
         <v>620</v>
@@ -2381,68 +2375,63 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.56</v>
+        <v>2.0771999999999999</v>
       </c>
       <c r="B4">
-        <v>120</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.0499999999999998</v>
+        <v>2.7517</v>
       </c>
       <c r="B5">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2.71</v>
+        <v>3.3969</v>
       </c>
       <c r="B6">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3.32</v>
+        <v>4.0274000000000001</v>
       </c>
       <c r="B7">
-        <v>400</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4.04</v>
+        <v>4.6627999999999998</v>
       </c>
       <c r="B8">
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4.5999999999999996</v>
+        <v>4.8094000000000001</v>
       </c>
       <c r="B9">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4.75</v>
-      </c>
-      <c r="B10">
         <v>620</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
       <c r="N23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
@@ -2455,40 +2444,35 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>2</v>
+      <c r="B25">
+        <v>0.83579999999999999</v>
       </c>
       <c r="C25">
-        <f>151.6*B26-117.58</f>
-        <v>631.32399999999996</v>
+        <f>151.6*B25-117.58</f>
+        <v>9.1272799999999989</v>
       </c>
       <c r="N25">
-        <v>4.9400000000000004</v>
+        <v>0.83579999999999999</v>
       </c>
       <c r="O25">
         <f>152.33*N25-132.53</f>
-        <v>619.9802000000002</v>
+        <v>-5.2125859999999875</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>4.9400000000000004</v>
+        <v>4.7653999999999996</v>
       </c>
       <c r="C26">
-        <f>151.6*B27-117.58</f>
-        <v>617.67999999999984</v>
+        <f>151.6*B26-117.58</f>
+        <v>604.8546399999999</v>
       </c>
       <c r="N26">
-        <v>4.8899999999999997</v>
+        <v>4.7653999999999996</v>
       </c>
       <c r="O26">
         <f>152.33*N26-132.53</f>
-        <v>612.36369999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>4.8499999999999996</v>
+        <v>593.38338199999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Collected more data for a 20mm 39cm flexor
</commit_message>
<xml_diff>
--- a/Testing_Data/PressureSensorCalibration.xlsx
+++ b/Testing_Data/PressureSensorCalibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C834A916-5249-4783-9E81-EE8B47AA3E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0294E47-96A7-4862-B733-03EAC2DAACCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED23B71C-6DC7-4F03-A302-FE33CB0246DD}"/>
   </bookViews>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -232,65 +224,59 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$14</c:f>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.82599999999999996</c:v>
+                  <c:v>0.83089999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4052</c:v>
+                  <c:v>2.0821000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1017000000000001</c:v>
+                  <c:v>2.7664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7566000000000002</c:v>
+                  <c:v>3.4310999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4310999999999998</c:v>
+                  <c:v>4.0468999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0225</c:v>
+                  <c:v>4.6773999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6449999999999996</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.8192000000000004</c:v>
+                  <c:v>4.8728999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>500</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>620</c:v>
                 </c:pt>
               </c:numCache>
@@ -616,10 +602,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.82599999999999996</c:v>
+                  <c:v>0.83089999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8192000000000004</c:v>
+                  <c:v>4.8728999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2322,7 +2308,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,13 +2333,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.82599999999999996</v>
+        <v>0.83089999999999997</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>0.82599999999999996</v>
+        <v>0.83089999999999997</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2361,13 +2347,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.4052</v>
+        <v>2.0821000000000001</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="M3">
-        <v>4.8192000000000004</v>
+        <v>4.8728999999999996</v>
       </c>
       <c r="N3">
         <v>620</v>
@@ -2375,66 +2361,67 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2.1017000000000001</v>
+        <v>2.7664</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.7566000000000002</v>
+        <v>3.4310999999999998</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3.4310999999999998</v>
+        <v>4.0468999999999999</v>
       </c>
       <c r="B6">
-        <v>400</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4.0225</v>
+        <v>4.6773999999999996</v>
       </c>
       <c r="B7">
-        <v>500</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4.6449999999999996</v>
+        <v>4.8728999999999996</v>
       </c>
       <c r="B8">
-        <v>600</v>
+        <v>620</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4.8192000000000004</v>
-      </c>
-      <c r="B9">
-        <v>620</v>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3</v>
       </c>
       <c r="N23" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3</v>
+      <c r="B24">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="C24">
+        <f>154.1*B24-125.6</f>
+        <v>2.457099999999997</v>
       </c>
       <c r="N24" t="s">
         <v>2</v>
@@ -2445,34 +2432,27 @@
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>0.83579999999999999</v>
+        <v>4.8239999999999998</v>
       </c>
       <c r="C25">
-        <f>151.6*B25-117.58</f>
-        <v>9.1272799999999989</v>
+        <f>154.1*B25-125.6</f>
+        <v>617.77839999999992</v>
       </c>
       <c r="N25">
         <v>0.83579999999999999</v>
       </c>
       <c r="O25">
-        <f>152.33*N25-132.53</f>
-        <v>-5.2125859999999875</v>
+        <f>153.39*N25-127.45</f>
+        <v>0.75336199999999565</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>4.7653999999999996</v>
-      </c>
-      <c r="C26">
-        <f>151.6*B26-117.58</f>
-        <v>604.8546399999999</v>
-      </c>
       <c r="N26">
         <v>4.7653999999999996</v>
       </c>
       <c r="O26">
-        <f>152.33*N26-132.53</f>
-        <v>593.38338199999998</v>
+        <f>153.39*N26-127.45</f>
+        <v>603.51470599999982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>